<commit_message>
Updated the excel test documents to include multiple sheets with data.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="188" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="188" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="2ndsheet" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>header1</t>
   </si>
@@ -80,19 +80,46 @@
   </si>
   <si>
     <t>not blank</t>
+  </si>
+  <si>
+    <t>column 1</t>
+  </si>
+  <si>
+    <t>column 2</t>
+  </si>
+  <si>
+    <t>last column</t>
+  </si>
+  <si>
+    <t>data 1,1</t>
+  </si>
+  <si>
+    <t>data 1,2</t>
+  </si>
+  <si>
+    <t>data 1,3</t>
+  </si>
+  <si>
+    <t>data 2,1</t>
+  </si>
+  <si>
+    <t>data 2,2</t>
+  </si>
+  <si>
+    <t>data 2,3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;" numFmtId="165"/>
   </numFmts>
   <fonts count="5">
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -113,6 +140,7 @@
     </font>
     <font>
       <name val="Arial"/>
+      <charset val="1"/>
       <family val="2"/>
       <b val="true"/>
       <sz val="10"/>
@@ -160,10 +188,9 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -183,14 +210,14 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="C9" activeCellId="0" pane="topLeft" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6235294117647"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.7490196078431"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6745098039216"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -258,7 +285,8 @@
       <c r="B7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2" t="b">
+      <c r="C7" s="0" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
@@ -301,19 +329,53 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6745098039216"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
+      <c r="A2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
+      <c r="A3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -328,17 +390,17 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6235294117647"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6745098039216"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Minor fix for test.xlsx.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="188" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="188" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>header1</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>header3</t>
+  </si>
+  <si>
+    <t>header4</t>
   </si>
   <si>
     <t>data1</t>
@@ -210,14 +213,14 @@
   </sheetPr>
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C9" activeCellId="0" pane="topLeft" sqref="C9"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="D2" activeCellId="0" pane="topLeft" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6745098039216"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8941176470588"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0274509803922"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.7294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -230,46 +233,49 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="A5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="A6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>1.2346</v>
@@ -280,10 +286,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
       <c r="A7" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" s="0" t="b">
         <f aca="false">TRUE()</f>
@@ -292,10 +298,10 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
       <c r="A8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="n">
         <f aca="false">AVERAGE(2,4,8,16,32,64,128)</f>
@@ -304,13 +310,13 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -331,45 +337,45 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B3" activeCellId="0" pane="topLeft" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -395,7 +401,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6745098039216"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7294117647059"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Updated the test spreadsheets to include date values.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>header1</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>not blank</t>
+  </si>
+  <si>
+    <t>data8</t>
+  </si>
+  <si>
+    <t>row with two dates</t>
   </si>
   <si>
     <t>column 1</t>
@@ -116,8 +122,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
+    <numFmt formatCode="MM/DD/YY" numFmtId="165"/>
+    <numFmt formatCode="MM/DD/YYYY\ HH:MM:SS" numFmtId="166"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -191,9 +199,11 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="165" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="166" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -211,16 +221,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D2" activeCellId="0" pane="topLeft" sqref="D2"/>
+      <selection activeCell="A10" activeCellId="0" pane="topLeft" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7294117647059"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0274509803922"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.7294117647059"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.7843137254902"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.1647058823529"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.7843137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.043137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.7843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
@@ -317,6 +329,20 @@
       </c>
       <c r="D9" s="0" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
+      <c r="A10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>40909</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>40953.0930555556</v>
       </c>
     </row>
   </sheetData>
@@ -342,40 +368,40 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7843137254902"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2">
       <c r="A2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="3">
       <c r="A3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -401,7 +427,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7294117647059"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7843137254902"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>